<commit_message>
feat: v0.0.15 + v2.2.9 LT
</commit_message>
<xml_diff>
--- a/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/LongTerm/Binance_BTC-USDT_1w/equity_curve.xlsx
+++ b/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/LongTerm/Binance_BTC-USDT_1w/equity_curve.xlsx
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C337"/>
+  <dimension ref="A1:C339"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,7 +400,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -424,7 +424,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>1600</v>
+        <v>1113.65260335</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1600</v>
+        <v>1159.57157768</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1600</v>
+        <v>1202.10546284</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1600</v>
+        <v>1429.32218897</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -496,23 +496,26 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1600</v>
+        <v>1132.69494239</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.2075300088874686</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1600</v>
+        <v>1563.32635826</v>
       </c>
       <c r="B15">
         <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1600</v>
+        <v>1774.10461568</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -520,7 +523,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>1600</v>
+        <v>2168.07675737</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -528,7 +531,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>1600</v>
+        <v>2890.23429284</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -536,7 +539,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>1600</v>
+        <v>3655.991187680001</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -544,1257 +547,1242 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>1600</v>
+        <v>2619.51876026</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.283499706157038</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>1600</v>
+        <v>2661.35650982</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.2720560928078085</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>1600</v>
+        <v>3131.95771139</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.1433355414137468</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>1600</v>
+        <v>2262.558928562391</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.3811366569518037</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>1600</v>
+        <v>2176.888201847391</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.4045696255551455</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>1600</v>
+        <v>2048.876718719421</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>0.4395837917706835</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>1600</v>
+        <v>2075.466143999421</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.4323109555095893</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>1600</v>
+        <v>1918.190300879421</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>0.4753296158526421</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>1600</v>
+        <v>1937.645491799421</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.4700081613082329</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>1600</v>
+        <v>2064.537487799421</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.4353002012815234</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>1600</v>
+        <v>2105.539641959421</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.4240851430236779</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>1600</v>
+        <v>2200.700363861321</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>0.39805643643856</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>1600</v>
+        <v>2249.221071978201</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>0.3847848759708035</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>1600</v>
+        <v>2049.645607778201</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>0.4393734824402424</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>1600</v>
+        <v>2018.520150158201</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>0.4478870307564656</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>1600</v>
+        <v>1776.414916098201</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.5141085344832385</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>1600</v>
+        <v>1852.892690478201</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>0.4931900556210039</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>1600</v>
+        <v>1659.437160098201</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.5461047155446681</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>1600</v>
+        <v>1595.164608378201</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.5636847775362248</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>1600</v>
+        <v>1531.450452218201</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>0.5811121051443178</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>1600</v>
+        <v>1576.252525178201</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>0.5688576792827417</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>1600</v>
+        <v>1648.658495438201</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>0.5490529350853283</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>1600</v>
+        <v>1575.478107978201</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>0.5690695006904654</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>1600</v>
+        <v>1787.786621298201</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>0.5109981043382423</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>1600</v>
+        <v>1954.125322038201</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.4655005382334525</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>1600</v>
+        <v>1712.260564898201</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.5316562658388796</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>1600</v>
+        <v>1566.372592058201</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>0.571560074505491</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>1600</v>
+        <v>1600.854536858201</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>0.5621284476142124</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>1600</v>
+        <v>1646.192588038201</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>0.5497274190415012</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>1600</v>
+        <v>1768.878613978201</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>0.5161698912352448</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>1600</v>
+        <v>1554.650361178201</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.5747663817087199</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>1600</v>
+        <v>1606.452758038201</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>0.5605972018062726</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>1600</v>
+        <v>1647.822940038201</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>0.549281479235767</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>1593.58402099648</v>
+        <v>1631.227994618201</v>
       </c>
       <c r="B60">
-        <v>0.004009986877199889</v>
+        <v>0.553820589033384</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>1592.74943347648</v>
+        <v>1628.923084478201</v>
       </c>
       <c r="B61">
-        <v>0.00453160407719988</v>
+        <v>0.5544510364337408</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>1572.38874483648</v>
+        <v>1572.692243998201</v>
       </c>
       <c r="B62">
-        <v>0.01725703447719995</v>
+        <v>0.5698315003335138</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>1590.89356467648</v>
+        <v>1623.797665378201</v>
       </c>
       <c r="B63">
-        <v>0.005691522077199918</v>
+        <v>0.5558529596980178</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>1575.48061374304</v>
+        <v>1603.381582458201</v>
       </c>
       <c r="B64">
-        <v>0.01532461641059979</v>
+        <v>0.5614372409153243</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>1574.87308542304</v>
+        <v>1602.550102938201</v>
       </c>
       <c r="B65">
-        <v>0.01570432161059987</v>
+        <v>0.5616646702162489</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>1569.50658526304</v>
+        <v>1595.205367178201</v>
       </c>
       <c r="B66">
-        <v>0.01905838421060002</v>
+        <v>0.5636736290410815</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>1452.19852502304</v>
+        <v>1434.654416038201</v>
       </c>
       <c r="B67">
-        <v>0.09237592186059984</v>
+        <v>0.6075881088355148</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>1217.49306214304</v>
+        <v>1113.430237358201</v>
       </c>
       <c r="B68">
-        <v>0.2390668361606</v>
+        <v>0.6954505139098117</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>1228.69511006304</v>
+        <v>1128.761659978201</v>
       </c>
       <c r="B69">
-        <v>0.2320655562105999</v>
+        <v>0.6912570074616387</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>1137.02385150304</v>
+        <v>1003.297921818201</v>
       </c>
       <c r="B70">
-        <v>0.2893600928105999</v>
+        <v>0.7255743052119148</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>1089.86595470304</v>
+        <v>938.7563620182009</v>
       </c>
       <c r="B71">
-        <v>0.3188337783105999</v>
+        <v>0.7432279472714178</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>1194.25361486304</v>
+        <v>1081.624107778201</v>
       </c>
       <c r="B72">
-        <v>0.2535914907105998</v>
+        <v>0.704150242094929</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>1175.22368366304</v>
+        <v>1055.579234578201</v>
       </c>
       <c r="B73">
-        <v>0.2654851977106</v>
+        <v>0.7112741304915331</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>1202.87366742304</v>
+        <v>1093.421742438201</v>
       </c>
       <c r="B74">
-        <v>0.2482039578605999</v>
+        <v>0.7009233101756849</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>1126.81499326304</v>
+        <v>989.3258051782011</v>
       </c>
       <c r="B75">
-        <v>0.2957406292106</v>
+        <v>0.729396009347057</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>1136.11702614304</v>
+        <v>1002.056816358201</v>
       </c>
       <c r="B76">
-        <v>0.2899268586605999</v>
+        <v>0.7259137768890299</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>1138.96291819796</v>
+        <v>1004.412674998201</v>
       </c>
       <c r="B77">
-        <v>0.288148176126275</v>
+        <v>0.725269393869744</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>1112.18601793796</v>
+        <v>985.5148573782012</v>
       </c>
       <c r="B78">
-        <v>0.3048837387887749</v>
+        <v>0.7304383936429606</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>1176.27674383796</v>
+        <v>1030.746935678201</v>
       </c>
       <c r="B79">
-        <v>0.2648270351012749</v>
+        <v>0.7180663511576222</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>1172.67299407796</v>
+        <v>1028.203586558201</v>
       </c>
       <c r="B80">
-        <v>0.267079378701275</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>0.7187620172545676</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81">
-        <v>1194.61313083796</v>
+        <v>1043.687854678201</v>
       </c>
       <c r="B81">
-        <v>0.2533667932262749</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>0.7145267039496068</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82">
-        <v>1213.14876361796</v>
+        <v>1056.769391538201</v>
       </c>
       <c r="B82">
-        <v>0.241782022738775</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>0.7109485944333471</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83">
-        <v>1244.64403495796</v>
+        <v>1078.997203118201</v>
       </c>
       <c r="B83">
-        <v>0.2220974781512749</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>0.7048687626069182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84">
-        <v>1263.21720679796</v>
+        <v>1092.105233198201</v>
       </c>
       <c r="B84">
-        <v>0.210489245751275</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>0.7012834065688152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85">
-        <v>1266.40513927796</v>
+        <v>1094.355118958201</v>
       </c>
       <c r="B85">
-        <v>0.208496787951275</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <v>0.700668009636902</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86">
-        <v>1298.68006801796</v>
+        <v>1117.133174338201</v>
       </c>
       <c r="B86">
-        <v>0.1883249574887751</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <v>0.694437673126038</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87">
-        <v>1606.59276385796</v>
+        <v>1334.442792418201</v>
       </c>
       <c r="B87">
-        <v>0</v>
-      </c>
-      <c r="C87" s="2">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>0.6349983564197252</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88">
-        <v>1595.33970871796</v>
+        <v>1326.500940238201</v>
       </c>
       <c r="B88">
-        <v>0.007004298409123755</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <v>0.6371706406984079</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89">
-        <v>1631.38875679796</v>
+        <v>1351.942583198201</v>
       </c>
       <c r="B89">
-        <v>0</v>
-      </c>
-      <c r="C89" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <v>0.6302117500299256</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90">
-        <v>1646.22534835796</v>
+        <v>1362.413518918201</v>
       </c>
       <c r="B90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+        <v>0.6273477016275977</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91">
-        <v>1781.39484055796</v>
+        <v>1457.809490318201</v>
       </c>
       <c r="B91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <v>0.6012546487445749</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92">
-        <v>2125.50962833796</v>
+        <v>1700.668762178201</v>
       </c>
       <c r="B92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>0.5348268978576498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93">
-        <v>2466.58663987796</v>
+        <v>1941.384121158201</v>
       </c>
       <c r="B93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>0.4689855578152654</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94">
-        <v>2601.13529377796</v>
+        <v>2036.341935458201</v>
       </c>
       <c r="B94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>0.4430123512550335</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95">
-        <v>2633.34669487796</v>
+        <v>2059.075156158201</v>
       </c>
       <c r="B95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+        <v>0.4367942780888271</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96">
-        <v>2316.329333177961</v>
+        <v>1835.339913258201</v>
       </c>
       <c r="B96">
-        <v>0.1203857290483703</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+        <v>0.4979911550544898</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97">
-        <v>2698.99673557796</v>
+        <v>2105.407722058201</v>
       </c>
       <c r="B97">
-        <v>0</v>
-      </c>
-      <c r="C97" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <v>0.424121226234618</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98">
-        <v>3262.87384345796</v>
+        <v>2503.364417618201</v>
       </c>
       <c r="B98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>0.3152706642034406</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99">
-        <v>3247.86688231796</v>
+        <v>2492.773243438201</v>
       </c>
       <c r="B99">
-        <v>0.004599307806548714</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+        <v>0.3181676006664415</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100">
-        <v>3407.30393299796</v>
+        <v>2605.296062598201</v>
       </c>
       <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+        <v>0.2873899501241808</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101">
-        <v>3051.53182327796</v>
+        <v>2354.209626958201</v>
       </c>
       <c r="B101">
-        <v>0.1044145508343218</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+        <v>0.3560680247557919</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102">
-        <v>3171.44601901796</v>
+        <v>2438.839161338201</v>
       </c>
       <c r="B102">
-        <v>0.06922127248345511</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <v>0.3329198468648863</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
       <c r="A103">
-        <v>2868.849431597961</v>
+        <v>2252.201760127744</v>
       </c>
       <c r="B103">
-        <v>0.1580294895871627</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>0.3839695873126723</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104">
-        <v>3269.56157137796</v>
+        <v>2456.831915217744</v>
       </c>
       <c r="B104">
-        <v>0.04042561636079411</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <v>0.3279984034160686</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105">
-        <v>3448.80769525796</v>
+        <v>2548.366856357744</v>
       </c>
       <c r="B105">
-        <v>0</v>
-      </c>
-      <c r="C105" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>0.3029614335654696</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106">
-        <v>3089.82166447796</v>
+        <v>2311.737604316184</v>
       </c>
       <c r="B106">
-        <v>0.1040898949725722</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>0.3676851267841391</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
       <c r="A107">
-        <v>3042.43870789796</v>
+        <v>2280.508323696184</v>
       </c>
       <c r="B107">
-        <v>0.117828833401975</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>0.3762270731447422</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108">
-        <v>2921.81993287796</v>
+        <v>2201.010591916184</v>
       </c>
       <c r="B108">
-        <v>0.152802884053117</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>0.3979715817332455</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
       <c r="A109">
-        <v>3111.30555727796</v>
+        <v>2325.897263516184</v>
       </c>
       <c r="B109">
-        <v>0.09786052682614288</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>0.3638121253262266</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110">
-        <v>3088.44426973796</v>
+        <v>2310.829787456184</v>
       </c>
       <c r="B110">
-        <v>0.1044892778497022</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>0.3679334361518037</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111">
-        <v>3009.57181705796</v>
+        <v>2258.846328936184</v>
       </c>
       <c r="B111">
-        <v>0.127358761929214</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <v>0.3821521406976938</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
       <c r="A112">
-        <v>2436.36480895796</v>
+        <v>1881.055583036184</v>
       </c>
       <c r="B112">
-        <v>0.2935631603038024</v>
+        <v>0.4854868388701302</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>2381.62419661796</v>
+        <v>1844.976999776184</v>
       </c>
       <c r="B113">
-        <v>0.3094354898672244</v>
+        <v>0.4953551841171259</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>2503.123695737961</v>
+        <v>1925.055201456184</v>
       </c>
       <c r="B114">
-        <v>0.2742060686133053</v>
+        <v>0.4734519032914367</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>2488.206250817961</v>
+        <v>1915.223373576184</v>
       </c>
       <c r="B115">
-        <v>0.2785314605278824</v>
+        <v>0.4761411405940679</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>2865.49690477796</v>
+        <v>2163.889066016184</v>
       </c>
       <c r="B116">
-        <v>0.1691340434208727</v>
+        <v>0.4081251964424637</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>2768.69810713796</v>
+        <v>2100.090666056184</v>
       </c>
       <c r="B117">
-        <v>0.1972013658677279</v>
+        <v>0.4255755667209778</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>2723.87069425796</v>
+        <v>2070.545699736184</v>
       </c>
       <c r="B118">
-        <v>0.210199310908745</v>
+        <v>0.4336568133113855</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>2568.78528691796</v>
+        <v>1968.331611476184</v>
       </c>
       <c r="B119">
-        <v>0.2551671435754486</v>
+        <v>0.4616147823033355</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>2107.02019747796</v>
+        <v>1663.990291316184</v>
       </c>
       <c r="B120">
-        <v>0.389058369251765</v>
+        <v>0.5448593265422748</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>2247.82343629796</v>
+        <v>1756.791251296184</v>
       </c>
       <c r="B121">
-        <v>0.348231726753373</v>
+        <v>0.5194760706162972</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>2282.24964193796</v>
+        <v>1779.480963256184</v>
       </c>
       <c r="B122">
-        <v>0.3382496666671191</v>
+        <v>0.5132698981188197</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>2169.19354369796</v>
+        <v>1704.967659896184</v>
       </c>
       <c r="B123">
-        <v>0.371030879257038</v>
+        <v>0.5336510477263723</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>2279.74607539796</v>
+        <v>1777.830906196184</v>
       </c>
       <c r="B124">
-        <v>0.3389755890035375</v>
+        <v>0.5137212277241974</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>2247.05821699796</v>
+        <v>1756.286908596184</v>
       </c>
       <c r="B125">
-        <v>0.3484536061295562</v>
+        <v>0.5196140202649998</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>2238.54262561796</v>
+        <v>1750.674430776184</v>
       </c>
       <c r="B126">
-        <v>0.3509227468101773</v>
+        <v>0.5211491656009385</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>2477.12645287796</v>
+        <v>1907.920871916184</v>
       </c>
       <c r="B127">
-        <v>0.2817441064388837</v>
+        <v>0.4781385473943381</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>2626.335553517961</v>
+        <v>2006.261988876184</v>
       </c>
       <c r="B128">
-        <v>0.2384801399251346</v>
+        <v>0.451239927591481</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129">
-        <v>2601.29988811796</v>
+        <v>1989.761418276184</v>
       </c>
       <c r="B129">
-        <v>0.2457393632893204</v>
+        <v>0.4557532236452583</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130">
-        <v>2808.20074873796</v>
+        <v>2126.126168456184</v>
       </c>
       <c r="B130">
-        <v>0.1857473663726804</v>
+        <v>0.4184542414596546</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131">
-        <v>3045.05489161796</v>
+        <v>2282.232604776184</v>
       </c>
       <c r="B131">
-        <v>0.1170702571196278</v>
+        <v>0.3757554415155933</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132">
-        <v>2977.34597785796</v>
+        <v>2237.606840136184</v>
       </c>
       <c r="B132">
-        <v>0.1367028141488578</v>
+        <v>0.3879616428845627</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133">
-        <v>2982.86999491796</v>
+        <v>2241.247623476184</v>
       </c>
       <c r="B133">
-        <v>0.1351010962370139</v>
+        <v>0.3869658025903441</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134">
-        <v>2577.29799067796</v>
+        <v>1973.942186116184</v>
       </c>
       <c r="B134">
-        <v>0.2526988401754926</v>
+        <v>0.460080157532109</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135">
-        <v>2433.32992033796</v>
+        <v>1879.055340856184</v>
       </c>
       <c r="B135">
-        <v>0.294443142282552</v>
+        <v>0.4860339523825316</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136">
-        <v>1847.287157051963</v>
+        <v>1370.523741676184</v>
       </c>
       <c r="B136">
-        <v>0.4643693356425918</v>
+        <v>0.6251293640163602</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137">
-        <v>1915.022097611963</v>
+        <v>1457.097496696184</v>
       </c>
       <c r="B137">
-        <v>0.4447292320052872</v>
+        <v>0.6014493958283249</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138">
-        <v>1924.735105531963</v>
+        <v>1469.511939836184</v>
       </c>
       <c r="B138">
-        <v>0.4419128940768619</v>
+        <v>0.5980537522113945</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139">
-        <v>2057.462174971963</v>
+        <v>1639.153792316184</v>
       </c>
       <c r="B139">
-        <v>0.403427979530163</v>
+        <v>0.5516526960349843</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140">
-        <v>2076.970088011963</v>
+        <v>1664.087353496184</v>
       </c>
       <c r="B140">
-        <v>0.3977715571477777</v>
+        <v>0.5448327777419585</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141">
-        <v>2109.274810811963</v>
+        <v>1705.376843596184</v>
       </c>
       <c r="B141">
-        <v>0.38840463221183</v>
+        <v>0.533539126313274</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142">
-        <v>2233.748185630963</v>
+        <v>1814.307254076184</v>
       </c>
       <c r="B142">
-        <v>0.3523129199977368</v>
+        <v>0.503744084452376</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143">
-        <v>2572.867316217663</v>
+        <v>2042.890591156184</v>
       </c>
       <c r="B143">
-        <v>0.2539835376280032</v>
+        <v>0.4412211391426929</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144">
-        <v>2524.404737037663</v>
+        <v>2010.271989136184</v>
       </c>
       <c r="B144">
-        <v>0.2680355183303875</v>
+        <v>0.4501430977431179</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <v>2795.084316777663</v>
+        <v>2192.457700996184</v>
       </c>
       <c r="B145">
-        <v>0.1895505450707364</v>
+        <v>0.4003109995493556</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>2523.717625377663</v>
+        <v>2009.809516396184</v>
       </c>
       <c r="B146">
-        <v>0.2682347499839659</v>
+        <v>0.4502695949681547</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>2729.548568037663</v>
+        <v>2148.347698136184</v>
       </c>
       <c r="B147">
-        <v>0.2085529814287017</v>
+        <v>0.4123761278813499</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>2814.015232677663</v>
+        <v>2205.199491096184</v>
       </c>
       <c r="B148">
-        <v>0.1840614260554809</v>
+        <v>0.3968258188019462</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <v>2699.527726497663</v>
+        <v>2128.141636076184</v>
       </c>
       <c r="B149">
-        <v>0.2172576829350448</v>
+        <v>0.4179029634295566</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <v>2686.121980077663</v>
+        <v>2119.118659696184</v>
       </c>
       <c r="B150">
-        <v>0.2211447498881929</v>
+        <v>0.4203709607295516</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <v>2635.694204997663</v>
+        <v>2085.177347576184</v>
       </c>
       <c r="B151">
-        <v>0.2357665495174784</v>
+        <v>0.4296547118048758</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>2622.421356717663</v>
+        <v>2076.243820656184</v>
       </c>
       <c r="B152">
-        <v>0.2396150819532679</v>
+        <v>0.4320982425634029</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <v>2688.401041797663</v>
+        <v>2120.652622776184</v>
       </c>
       <c r="B153">
-        <v>0.2204839239096573</v>
+        <v>0.4199513855716112</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
-        <v>2661.889276677663</v>
+        <v>2102.808407096184</v>
       </c>
       <c r="B154">
-        <v>0.2281711501810592</v>
+        <v>0.4248322003121203</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <v>2866.198959777663</v>
+        <v>2240.322677996184</v>
       </c>
       <c r="B155">
-        <v>0.1689304788670507</v>
+        <v>0.3872187970404173</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <v>3188.493914997664</v>
+        <v>2457.249037576184</v>
       </c>
       <c r="B156">
-        <v>0.07547935497192915</v>
+        <v>0.327884310592255</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <v>3361.072046457663</v>
+        <v>2573.405822516184</v>
       </c>
       <c r="B157">
-        <v>0.02543941458983978</v>
+        <v>0.2961126845195702</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <v>3425.915028297663</v>
+        <v>2617.049546276184</v>
       </c>
       <c r="B158">
-        <v>0.006637849652149086</v>
+        <v>0.2841750945420365</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <v>3351.585381357663</v>
+        <v>2567.020653616184</v>
       </c>
       <c r="B159">
-        <v>0.02819012322257786</v>
+        <v>0.2978591791286154</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <v>3369.407870217663</v>
+        <v>2579.016397156184</v>
       </c>
       <c r="B160">
-        <v>0.02302239847976162</v>
+        <v>0.2945780597483435</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161">
-        <v>2958.000470697663</v>
+        <v>2349.134200975368</v>
       </c>
       <c r="B161">
-        <v>0.1423121460889647</v>
+        <v>0.357456273720925</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162">
-        <v>2979.668522757663</v>
+        <v>2358.951346905369</v>
       </c>
       <c r="B162">
-        <v>0.1360293799927881</v>
+        <v>0.3547710522786299</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163">
-        <v>3145.777059657663</v>
+        <v>2434.210153855368</v>
       </c>
       <c r="B163">
-        <v>0.08786533271105768</v>
+        <v>0.3341859898190683</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164">
-        <v>3104.485324797663</v>
+        <v>2415.502104525368</v>
       </c>
       <c r="B164">
-        <v>0.09983808924276427</v>
+        <v>0.339303083479754</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165">
-        <v>3074.054478357663</v>
+        <v>2401.714798705369</v>
       </c>
       <c r="B165">
-        <v>0.1086616738345761</v>
+        <v>0.343074237487581</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>3272.663679537663</v>
+        <v>2523.799263227649</v>
       </c>
       <c r="B166">
-        <v>0.05107388735025464</v>
+        <v>0.3096812509471097</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167">
-        <v>3310.587718977663</v>
+        <v>2552.549938185869</v>
       </c>
       <c r="B167">
-        <v>0.04007761188608638</v>
+        <v>0.3018172618174028</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168">
-        <v>3741.994874757663</v>
+        <v>2885.235796825868</v>
       </c>
       <c r="B168">
-        <v>0</v>
-      </c>
-      <c r="C168" s="2">
-        <v>441</v>
+        <v>0.2108198163746763</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>3949.166109297663</v>
+        <v>3044.998886345868</v>
       </c>
       <c r="B169">
-        <v>0</v>
+        <v>0.1671208353545984</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>4433.707072497663</v>
+        <v>3418.659647945869</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>0.06491578550131483</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>4569.970080297663</v>
+        <v>3523.740834345868</v>
       </c>
       <c r="B171">
-        <v>0</v>
+        <v>0.03617359740356896</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172">
-        <v>5264.837901957663</v>
+        <v>4059.598190425868</v>
       </c>
       <c r="B172">
         <v>0</v>
+      </c>
+      <c r="C172" s="2">
+        <v>1071</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173">
-        <v>5199.960988677663</v>
+        <v>4009.567421785869</v>
       </c>
       <c r="B173">
-        <v>0.01232268010680371</v>
+        <v>0.01232406910565476</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174">
-        <v>5532.039509097664</v>
+        <v>4265.654568745869</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -1805,15 +1793,15 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175">
-        <v>5479.895368677664</v>
+        <v>4225.442861785869</v>
       </c>
       <c r="B175">
-        <v>0.009425843820212498</v>
+        <v>0.009426854967260589</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176">
-        <v>6690.266592537663</v>
+        <v>5158.838111465869</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -1824,7 +1812,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177">
-        <v>7489.391591217663</v>
+        <v>5775.094895305869</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -1832,7 +1820,7 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178">
-        <v>9389.096984397664</v>
+        <v>7240.080145145869</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -1840,7 +1828,7 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179">
-        <v>10845.31280153766</v>
+        <v>8363.062003465868</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -1848,31 +1836,31 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180">
-        <v>10188.90626711767</v>
+        <v>7856.864624505869</v>
       </c>
       <c r="B180">
-        <v>0.06052444465473905</v>
+        <v>0.06052775631105178</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181">
-        <v>9179.810690097664</v>
+        <v>7078.685996745869</v>
       </c>
       <c r="B181">
-        <v>0.1535688404675486</v>
+        <v>0.1535772431422511</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182">
-        <v>9415.374057057663</v>
+        <v>7260.344089225869</v>
       </c>
       <c r="B182">
-        <v>0.1318485479070057</v>
+        <v>0.1318557621338936</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183">
-        <v>11027.88374207767</v>
+        <v>8503.854220985868</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -1883,7 +1871,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184">
-        <v>13793.88990227766</v>
+        <v>10636.89981858587</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -1891,7 +1879,7 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185">
-        <v>16290.89891663766</v>
+        <v>12562.50438226587</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -1899,23 +1887,23 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>12820.58633921767</v>
+        <v>9886.32271930587</v>
       </c>
       <c r="B186">
-        <v>0.2130215524126673</v>
+        <v>0.2130293117937446</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>14470.81081979767</v>
+        <v>11158.91716034587</v>
       </c>
       <c r="B187">
-        <v>0.1117242275060196</v>
+        <v>0.1117282970982604</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>16731.93411851766</v>
+        <v>12902.61504770587</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -1926,31 +1914,31 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189">
-        <v>16274.77865501766</v>
+        <v>12550.07300970587</v>
       </c>
       <c r="B189">
-        <v>0.0273223322696482</v>
+        <v>0.02732330126075355</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>15829.73106035766</v>
+        <v>12206.86812962587</v>
       </c>
       <c r="B190">
-        <v>0.05392102621068251</v>
+        <v>0.0539229385289387</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191">
-        <v>16515.25359791766</v>
+        <v>12735.51873490587</v>
       </c>
       <c r="B191">
-        <v>0.01295011796395928</v>
+        <v>0.01295057724206927</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192">
-        <v>17024.34395795766</v>
+        <v>13128.11111842587</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -1961,215 +1949,215 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <v>15935.02597391766</v>
+        <v>12477.95843323403</v>
       </c>
       <c r="B193">
-        <v>0.06398590082120736</v>
+        <v>0.04952370370169423</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <v>13932.15486503766</v>
+        <v>12356.59506353588</v>
       </c>
       <c r="B194">
-        <v>0.1816333775067217</v>
+        <v>0.0587682453271694</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <v>16056.10466231766</v>
+        <v>12484.77027569588</v>
       </c>
       <c r="B195">
-        <v>0.05687380953011212</v>
+        <v>0.0490048291735613</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <v>16526.23324637766</v>
+        <v>12513.14139401588</v>
       </c>
       <c r="B196">
-        <v>0.02925873166156101</v>
+        <v>0.04684373241987994</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <v>13187.00064929766</v>
+        <v>12311.62681625588</v>
       </c>
       <c r="B197">
-        <v>0.2254033000118231</v>
+        <v>0.06219358556647347</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <v>9857.124646797663</v>
+        <v>12110.67688625588</v>
       </c>
       <c r="B198">
-        <v>0.4209982674727291</v>
+        <v>0.07750042812647884</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <v>10135.93363403766</v>
+        <v>12127.50233153588</v>
       </c>
       <c r="B199">
-        <v>0.4046211907449252</v>
+        <v>0.07621879323413061</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200">
-        <v>10179.77305451766</v>
+        <v>12130.14793409588</v>
       </c>
       <c r="B200">
-        <v>0.402046088844478</v>
+        <v>0.07601727128355185</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201">
-        <v>11091.47126063766</v>
+        <v>12185.16670673588</v>
       </c>
       <c r="B201">
-        <v>0.3484934698201281</v>
+        <v>0.07182635820064998</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202">
-        <v>10124.30928821766</v>
+        <v>12126.80083049588</v>
       </c>
       <c r="B202">
-        <v>0.4053039980148384</v>
+        <v>0.07627222826630475</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203">
-        <v>9869.874385377663</v>
+        <v>12098.4400809322</v>
       </c>
       <c r="B203">
-        <v>0.4202493552907686</v>
+        <v>0.07843253520672022</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204">
-        <v>10035.62098691766</v>
+        <v>12116.5925934922</v>
       </c>
       <c r="B204">
-        <v>0.4105134969252822</v>
+        <v>0.07704981438753689</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205">
-        <v>9745.077376677662</v>
+        <v>12084.7723541322</v>
       </c>
       <c r="B205">
-        <v>0.4275798585400093</v>
+        <v>0.0794736390393056</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206">
-        <v>9043.706029017665</v>
+        <v>12007.9583978922</v>
       </c>
       <c r="B206">
-        <v>0.4687780009995405</v>
+        <v>0.08532474401145862</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207">
-        <v>10062.34482353766</v>
+        <v>12119.5193791722</v>
       </c>
       <c r="B207">
-        <v>0.4089437544032798</v>
+        <v>0.07682687403811428</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208">
-        <v>11324.71315157766</v>
+        <v>12257.7735377322</v>
       </c>
       <c r="B208">
-        <v>0.3347929776592554</v>
+        <v>0.06629572014149965</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209">
-        <v>12441.32049623767</v>
+        <v>12428.56649636799</v>
       </c>
       <c r="B209">
-        <v>0.2692041157672781</v>
+        <v>0.05328600708414488</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210">
-        <v>13340.34813713766</v>
+        <v>12601.96530438127</v>
       </c>
       <c r="B210">
-        <v>0.2163957583280615</v>
+        <v>0.04007780017234408</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211">
-        <v>13980.91717193766</v>
+        <v>12749.24238323993</v>
       </c>
       <c r="B211">
-        <v>0.1787691081392547</v>
+        <v>0.02885934859693429</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212">
-        <v>13847.62599275766</v>
+        <v>12713.26024862049</v>
       </c>
       <c r="B212">
-        <v>0.1865985539909812</v>
+        <v>0.03160019488432875</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213">
-        <v>14692.81574885766</v>
+        <v>12968.12567314449</v>
       </c>
       <c r="B213">
-        <v>0.1369526023944188</v>
+        <v>0.01218647860596145</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214">
-        <v>13072.12575917766</v>
+        <v>12408.37236572626</v>
       </c>
       <c r="B214">
-        <v>0.2321509838229402</v>
+        <v>0.05482424289427479</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215">
-        <v>13416.10855979766</v>
+        <v>12504.49517516284</v>
       </c>
       <c r="B215">
-        <v>0.2119456354424399</v>
+        <v>0.04750233583777019</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216">
-        <v>12262.19925209766</v>
+        <v>12180.38590646284</v>
       </c>
       <c r="B216">
-        <v>0.2797255928111131</v>
+        <v>0.07219052332919818</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217">
-        <v>13687.06807391766</v>
+        <v>12580.60210088284</v>
       </c>
       <c r="B217">
-        <v>0.196029632171527</v>
+        <v>0.04170508709166665</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218">
-        <v>15513.42500429766</v>
+        <v>13093.58800466284</v>
       </c>
       <c r="B218">
-        <v>0.08875049502002996</v>
+        <v>0.002629709137255465</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219">
-        <v>17455.81049375766</v>
+        <v>13700.87750184828</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -2180,23 +2168,23 @@
     </row>
     <row r="220" spans="1:3">
       <c r="A220">
-        <v>17264.63227793766</v>
+        <v>13635.12242143388</v>
       </c>
       <c r="B220">
-        <v>0.01095212484624319</v>
+        <v>0.004799333502947589</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221">
-        <v>17391.19089389766</v>
+        <v>13681.4698295364</v>
       </c>
       <c r="B221">
-        <v>0.003701896275919436</v>
+        <v>0.001416527686585178</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222">
-        <v>17949.30370187766</v>
+        <v>13903.48404710065</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -2207,7 +2195,7 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223">
-        <v>18584.24860049766</v>
+        <v>14173.69659416431</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -2215,850 +2203,850 @@
     </row>
     <row r="224" spans="1:3">
       <c r="A224">
-        <v>16634.01646553766</v>
+        <v>13535.91812131227</v>
       </c>
       <c r="B224">
-        <v>0.1049400584809103</v>
+        <v>0.0449973278752579</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225">
-        <v>16253.09646485766</v>
+        <v>13471.41571097227</v>
       </c>
       <c r="B225">
-        <v>0.1254369862216314</v>
+        <v>0.04954818092276558</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226">
-        <v>12252.96931717717</v>
+        <v>13094.18285842227</v>
       </c>
       <c r="B226">
-        <v>0.3406798638687465</v>
+        <v>0.07616317511597526</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227">
-        <v>12252.96931717717</v>
+        <v>13125.66796759227</v>
       </c>
       <c r="B227">
-        <v>0.3406798638687465</v>
+        <v>0.07394179913541676</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228">
-        <v>12252.96931717717</v>
+        <v>12964.18115532227</v>
       </c>
       <c r="B228">
-        <v>0.3406798638687465</v>
+        <v>0.08533521448032322</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229">
-        <v>12252.96931717717</v>
+        <v>13160.21841838227</v>
       </c>
       <c r="B229">
-        <v>0.3406798638687465</v>
+        <v>0.07150415341889815</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230">
-        <v>12252.96931717717</v>
+        <v>12993.14676627227</v>
       </c>
       <c r="B230">
-        <v>0.3406798638687465</v>
+        <v>0.08329159722369839</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231">
-        <v>12252.96931717717</v>
+        <v>12733.55705191227</v>
       </c>
       <c r="B231">
-        <v>0.3406798638687465</v>
+        <v>0.1016064886590688</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232">
-        <v>12252.96931717717</v>
+        <v>12791.35133415227</v>
       </c>
       <c r="B232">
-        <v>0.3406798638687465</v>
+        <v>0.09752891568041511</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233">
-        <v>12252.96931717717</v>
+        <v>12464.46248024227</v>
       </c>
       <c r="B233">
-        <v>0.3406798638687465</v>
+        <v>0.1205919784275455</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234">
-        <v>12252.96931717717</v>
+        <v>12542.85373225227</v>
       </c>
       <c r="B234">
-        <v>0.3406798638687465</v>
+        <v>0.1150612228134966</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235">
-        <v>12252.96931717717</v>
+        <v>12758.27561816227</v>
       </c>
       <c r="B235">
-        <v>0.3406798638687465</v>
+        <v>0.09986251410128288</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236">
-        <v>12252.96931717717</v>
+        <v>12742.60847615227</v>
       </c>
       <c r="B236">
-        <v>0.3406798638687465</v>
+        <v>0.1009678814912163</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237">
-        <v>12252.96931717717</v>
+        <v>12523.38712512177</v>
       </c>
       <c r="B237">
-        <v>0.3406798638687465</v>
+        <v>0.1164346547196456</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238">
-        <v>12252.96931717717</v>
+        <v>12472.99353645522</v>
       </c>
       <c r="B238">
-        <v>0.3406798638687465</v>
+        <v>0.1199900849020088</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239">
-        <v>12252.96931717717</v>
+        <v>12525.35288649522</v>
       </c>
       <c r="B239">
-        <v>0.3406798638687465</v>
+        <v>0.1162959639158464</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240">
-        <v>12244.18464683077</v>
+        <v>12478.67171187522</v>
       </c>
       <c r="B240">
-        <v>0.3411525582743823</v>
+        <v>0.119589471315971</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241">
-        <v>12289.07893874077</v>
+        <v>12731.47783629522</v>
       </c>
       <c r="B241">
-        <v>0.3387368409174374</v>
+        <v>0.1017531840256047</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242">
-        <v>12360.78120769077</v>
+        <v>13201.51403832366</v>
       </c>
       <c r="B242">
-        <v>0.3348786128829675</v>
+        <v>0.06859061426790547</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243">
-        <v>12350.42636253757</v>
+        <v>13161.03303298046</v>
       </c>
       <c r="B243">
-        <v>0.3354357968388969</v>
+        <v>0.0714466797321448</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244">
-        <v>12204.97670347581</v>
+        <v>12711.1401124187</v>
       </c>
       <c r="B244">
-        <v>0.3432622988508138</v>
+        <v>0.1031880760272365</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245">
-        <v>12090.71543861796</v>
+        <v>12419.11221649085</v>
       </c>
       <c r="B245">
-        <v>0.3494105842786567</v>
+        <v>0.1237915857741634</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246">
-        <v>12076.92078229571</v>
+        <v>12392.31905968085</v>
       </c>
       <c r="B246">
-        <v>0.3501528610647023</v>
+        <v>0.1256819293857961</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247">
-        <v>12019.64864599571</v>
+        <v>12276.94125586085</v>
       </c>
       <c r="B247">
-        <v>0.3532346179616944</v>
+        <v>0.1338222054989101</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248">
-        <v>11761.22751274571</v>
+        <v>11756.33796181085</v>
       </c>
       <c r="B248">
-        <v>0.3671400030437192</v>
+        <v>0.170552446660157</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249">
-        <v>11603.16824689572</v>
+        <v>11437.91905612085</v>
       </c>
       <c r="B249">
-        <v>0.3756450155006537</v>
+        <v>0.1930179272477055</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250">
-        <v>11542.79443864571</v>
+        <v>11316.29276707085</v>
       </c>
       <c r="B250">
-        <v>0.3788936702914847</v>
+        <v>0.2015990541430052</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251">
-        <v>11494.61906224571</v>
+        <v>11219.24087611085</v>
       </c>
       <c r="B251">
-        <v>0.3814859395532459</v>
+        <v>0.2084463780090994</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252">
-        <v>11520.93456409571</v>
+        <v>11272.25487220085</v>
       </c>
       <c r="B252">
-        <v>0.3800699284776464</v>
+        <v>0.204706069633102</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253">
-        <v>11325.82265629572</v>
+        <v>10879.19142328085</v>
       </c>
       <c r="B253">
-        <v>0.3905687068783386</v>
+        <v>0.232437963448427</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254">
-        <v>10975.78173874571</v>
+        <v>10174.01513821085</v>
       </c>
       <c r="B254">
-        <v>0.4094040617573422</v>
+        <v>0.2821904243103548</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255">
-        <v>11002.85326219571</v>
+        <v>10228.55218054085</v>
       </c>
       <c r="B255">
-        <v>0.4079473699086723</v>
+        <v>0.2783426601108265</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256">
-        <v>10902.38639179572</v>
+        <v>10026.15625798085</v>
       </c>
       <c r="B256">
-        <v>0.4133533926411335</v>
+        <v>0.2926223451044599</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257">
-        <v>10992.60963619571</v>
+        <v>10207.91584414085</v>
       </c>
       <c r="B257">
-        <v>0.4084985692721875</v>
+        <v>0.2797986201889121</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258">
-        <v>10988.85811234572</v>
+        <v>10200.35819725085</v>
       </c>
       <c r="B258">
-        <v>0.4087004350527549</v>
+        <v>0.2803318365478057</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259">
-        <v>11092.78308154571</v>
+        <v>10451.59199612685</v>
       </c>
       <c r="B259">
-        <v>0.4031083354508793</v>
+        <v>0.262606481894776</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260">
-        <v>11134.41327094572</v>
+        <v>10567.64826862299</v>
       </c>
       <c r="B260">
-        <v>0.4008682562152364</v>
+        <v>0.254418337628733</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261">
-        <v>11124.38857924571</v>
+        <v>10545.14710634299</v>
       </c>
       <c r="B261">
-        <v>0.4014076749410348</v>
+        <v>0.2560058671860725</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262">
-        <v>11238.04611984971</v>
+        <v>10777.43759704698</v>
       </c>
       <c r="B262">
-        <v>0.3952918753169947</v>
+        <v>0.2396170240102119</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263">
-        <v>10899.14371411346</v>
+        <v>10145.88626653073</v>
       </c>
       <c r="B263">
-        <v>0.4135278779136869</v>
+        <v>0.2841750069132941</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264">
-        <v>10615.76622437326</v>
+        <v>9702.504866530733</v>
       </c>
       <c r="B264">
-        <v>0.4287761398064283</v>
+        <v>0.3154569944353462</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265">
-        <v>10679.94166172325</v>
+        <v>9803.100414880731</v>
       </c>
       <c r="B265">
-        <v>0.4253229231211823</v>
+        <v>0.3083596541133151</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266">
-        <v>10943.54311127325</v>
+        <v>10216.29794743073</v>
       </c>
       <c r="B266">
-        <v>0.4111387903528043</v>
+        <v>0.2792072357724198</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267">
-        <v>10595.64438392325</v>
+        <v>9670.963709080732</v>
       </c>
       <c r="B267">
-        <v>0.4298588761000798</v>
+        <v>0.3176823248027952</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268">
-        <v>10507.78541192325</v>
+        <v>9533.244017080733</v>
       </c>
       <c r="B268">
-        <v>0.4345864803142017</v>
+        <v>0.3273988931718896</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269">
-        <v>10543.78045922326</v>
+        <v>9589.666562380731</v>
       </c>
       <c r="B269">
-        <v>0.4326496224904726</v>
+        <v>0.3234181006577315</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270">
-        <v>10598.94053852325</v>
+        <v>9676.130459680731</v>
       </c>
       <c r="B270">
-        <v>0.4296815132875789</v>
+        <v>0.317317793886977</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271">
-        <v>10573.53532592325</v>
+        <v>9636.307571080732</v>
       </c>
       <c r="B271">
-        <v>0.4310485426007425</v>
+        <v>0.3201274270927842</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272">
-        <v>10617.90064322325</v>
+        <v>9713.255069166651</v>
       </c>
       <c r="B272">
-        <v>0.4286612888433422</v>
+        <v>0.3146985329736874</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273">
-        <v>10770.45314342325</v>
+        <v>10005.78687935945</v>
       </c>
       <c r="B273">
-        <v>0.4204525899887694</v>
+        <v>0.2940594704504185</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274">
-        <v>10816.7657129857</v>
+        <v>10089.05587982189</v>
       </c>
       <c r="B274">
-        <v>0.4179605565168754</v>
+        <v>0.288184573953994</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275">
-        <v>9937.780904598036</v>
+        <v>8602.006887464233</v>
       </c>
       <c r="B275">
-        <v>0.4652578579726965</v>
+        <v>0.3931006755848077</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276">
-        <v>9928.254410418034</v>
+        <v>8585.886441104232</v>
       </c>
       <c r="B276">
-        <v>0.4657704691836629</v>
+        <v>0.3942380250583838</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277">
-        <v>9956.774376368034</v>
+        <v>8634.147068004233</v>
       </c>
       <c r="B277">
-        <v>0.4642358380794903</v>
+        <v>0.3908330822067165</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278">
-        <v>10086.73557024803</v>
+        <v>8854.063483764234</v>
       </c>
       <c r="B278">
-        <v>0.4572427550297661</v>
+        <v>0.3753172699202769</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279">
-        <v>10082.77099739803</v>
+        <v>8847.354753064232</v>
       </c>
       <c r="B279">
-        <v>0.4574560847658897</v>
+        <v>0.3757905925045041</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280">
-        <v>10016.18153263803</v>
+        <v>8724.130430995632</v>
       </c>
       <c r="B280">
-        <v>0.4610391978737405</v>
+        <v>0.3844844657823712</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281">
-        <v>10034.20929973804</v>
+        <v>8759.615465578634</v>
       </c>
       <c r="B281">
-        <v>0.460069141591803</v>
+        <v>0.3819808821655458</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282">
-        <v>9986.034243127155</v>
+        <v>8670.213182727752</v>
       </c>
       <c r="B282">
-        <v>0.4626613936460287</v>
+        <v>0.3882885015121947</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283">
-        <v>10113.90286375003</v>
+        <v>8881.202850207752</v>
       </c>
       <c r="B283">
-        <v>0.4557809098895078</v>
+        <v>0.3734025001025928</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284">
-        <v>11161.95742508302</v>
+        <v>10426.70587997775</v>
       </c>
       <c r="B284">
-        <v>0.3993861325776645</v>
+        <v>0.2643622776382339</v>
       </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285">
-        <v>11719.32298117218</v>
+        <v>11227.84169916691</v>
       </c>
       <c r="B285">
-        <v>0.3693948443598436</v>
+        <v>0.2078395622078072</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286">
-        <v>12055.67573162823</v>
+        <v>11701.50853252295</v>
       </c>
       <c r="B286">
-        <v>0.3512960361870433</v>
+        <v>0.1744208397024122</v>
       </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287">
-        <v>11774.74687577046</v>
+        <v>11313.13720111519</v>
       </c>
       <c r="B287">
-        <v>0.3664125395171934</v>
+        <v>0.2018216894967885</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288">
-        <v>11351.24695200103</v>
+        <v>10762.36714270519</v>
       </c>
       <c r="B288">
-        <v>0.3892006507221898</v>
+        <v>0.2406802931610412</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289">
-        <v>12323.06298321751</v>
+        <v>11954.70474916519</v>
       </c>
       <c r="B289">
-        <v>0.3369081931627023</v>
+        <v>0.156557030147854</v>
       </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290">
-        <v>12027.79584455858</v>
+        <v>11611.16649553519</v>
       </c>
       <c r="B290">
-        <v>0.3527962252809894</v>
+        <v>0.1807947617338005</v>
       </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291">
-        <v>11541.28603151068</v>
+        <v>11001.2427096274</v>
       </c>
       <c r="B291">
-        <v>0.3789748361845732</v>
+        <v>0.2238268516233862</v>
       </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292">
-        <v>11344.04996794436</v>
+        <v>10834.71469680108</v>
       </c>
       <c r="B292">
-        <v>0.3895879133019896</v>
+        <v>0.2355759399236739</v>
       </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293">
-        <v>14058.42540850436</v>
+        <v>13125.42070488108</v>
       </c>
       <c r="B293">
-        <v>0.2435300608210821</v>
+        <v>0.07395924431702827</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294">
-        <v>14055.6557452497</v>
+        <v>13122.99276998643</v>
       </c>
       <c r="B294">
-        <v>0.2436790936560485</v>
+        <v>0.07413054295309851</v>
       </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295">
-        <v>14154.9559303808</v>
+        <v>13207.84252475753</v>
       </c>
       <c r="B295">
-        <v>0.2383358491017089</v>
+        <v>0.0681441191428106</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296">
-        <v>14229.32491974081</v>
+        <v>13273.61654444163</v>
       </c>
       <c r="B296">
-        <v>0.2343341274847257</v>
+        <v>0.06350354995557528</v>
       </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297">
-        <v>15199.21620510081</v>
+        <v>14171.99397549187</v>
       </c>
       <c r="B297">
-        <v>0.1821452385923317</v>
+        <v>0.000120125237698443</v>
       </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298">
-        <v>13870.35218790081</v>
+        <v>12985.6564071028</v>
       </c>
       <c r="B298">
-        <v>0.253650094439149</v>
+        <v>0.0838200662169285</v>
       </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299">
-        <v>14674.6134665408</v>
+        <v>13350.2021168382</v>
       </c>
       <c r="B299">
-        <v>0.2103735920672176</v>
+        <v>0.05810019086094753</v>
       </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300">
-        <v>14281.39153590081</v>
+        <v>13157.6323095758</v>
       </c>
       <c r="B300">
-        <v>0.2315324744677398</v>
+        <v>0.0716866117345033</v>
       </c>
     </row>
     <row r="301" spans="1:2">
       <c r="A301">
-        <v>13540.84502838081</v>
+        <v>12795.9015428558</v>
       </c>
       <c r="B301">
-        <v>0.2713805481477363</v>
+        <v>0.09720788378352774</v>
       </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302">
-        <v>13457.6872882208</v>
+        <v>12755.2819290958</v>
       </c>
       <c r="B302">
-        <v>0.2758551837355196</v>
+        <v>0.1000737285185367</v>
       </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303">
-        <v>14102.62981350081</v>
+        <v>13070.3135331758</v>
       </c>
       <c r="B303">
-        <v>0.2411514655952699</v>
+        <v>0.07784723298245289</v>
       </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304">
-        <v>13637.58983454081</v>
+        <v>12843.1579576158</v>
       </c>
       <c r="B304">
-        <v>0.2661748060034232</v>
+        <v>0.09387379133657514</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305">
-        <v>13055.1037467008</v>
+        <v>12558.6341133758</v>
       </c>
       <c r="B305">
-        <v>0.2975178051400363</v>
+        <v>0.1139478660389466</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306">
-        <v>13258.01372478081</v>
+        <v>12657.7484582558</v>
       </c>
       <c r="B306">
-        <v>0.2865994203055499</v>
+        <v>0.1069550293980939</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307">
-        <v>15276.58169334081</v>
+        <v>13643.7474894158</v>
       </c>
       <c r="B307">
-        <v>0.1779822783401789</v>
+        <v>0.03738961824304199</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308">
-        <v>15352.16495022081</v>
+        <v>13682.68044381097</v>
       </c>
       <c r="B308">
-        <v>0.1739152181912968</v>
+        <v>0.03464277276511629</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309">
-        <v>15128.73972654081</v>
+        <v>13558.25823451863</v>
       </c>
       <c r="B309">
-        <v>0.1859375080606874</v>
+        <v>0.04342116084939129</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310">
-        <v>15163.6401252608</v>
+        <v>13578.29130670611</v>
       </c>
       <c r="B310">
-        <v>0.1840595521922396</v>
+        <v>0.04200776300681797</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311">
-        <v>15091.0582635008</v>
+        <v>13532.67708684011</v>
       </c>
       <c r="B311">
-        <v>0.1879651102441297</v>
+        <v>0.04522599330848687</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312">
-        <v>14698.05666366081</v>
+        <v>13300.78485214402</v>
       </c>
       <c r="B312">
-        <v>0.2091121368626541</v>
+        <v>0.06158673823875249</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313">
-        <v>14603.7208075808</v>
+        <v>13245.59934739401</v>
       </c>
       <c r="B313">
-        <v>0.2141882557904581</v>
+        <v>0.06548025355307929</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314">
-        <v>14709.19560966081</v>
+        <v>13307.30102089402</v>
       </c>
       <c r="B314">
-        <v>0.2085127612172109</v>
+        <v>0.06112700152104367</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="A315">
-        <v>13184.57991726081</v>
+        <v>12415.41653464402</v>
       </c>
       <c r="B315">
-        <v>0.2905508207144978</v>
+        <v>0.1240523280457566</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316">
-        <v>13141.38528798081</v>
+        <v>12390.14812114402</v>
       </c>
       <c r="B316">
-        <v>0.2928750809097066</v>
+        <v>0.1258350961000978</v>
       </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317">
-        <v>13077.4599785408</v>
+        <v>12352.75247314402</v>
       </c>
       <c r="B317">
-        <v>0.2963148384599952</v>
+        <v>0.1284734796545615</v>
       </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318">
-        <v>13014.00470814081</v>
+        <v>12315.63179314402</v>
       </c>
       <c r="B318">
-        <v>0.299729303675355</v>
+        <v>0.131092463329948</v>
       </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319">
-        <v>13349.8378097408</v>
+        <v>12512.09070064401</v>
       </c>
       <c r="B319">
-        <v>0.2816584572925206</v>
+        <v>0.1172316538936232</v>
       </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320">
-        <v>13213.16906262081</v>
+        <v>12426.43781369152</v>
       </c>
       <c r="B320">
-        <v>0.2890124671348306</v>
+        <v>0.1232747412691327</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321">
-        <v>14067.16634718081</v>
+        <v>12990.9590299529</v>
       </c>
       <c r="B321">
-        <v>0.2430597195732677</v>
+        <v>0.08344594907572511</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322">
-        <v>14030.1899427008</v>
+        <v>12964.66434033076</v>
       </c>
       <c r="B322">
-        <v>0.245049383254317</v>
+        <v>0.08530112421986979</v>
       </c>
     </row>
     <row r="323" spans="1:3">
       <c r="A323">
-        <v>13656.65579310081</v>
+        <v>12690.0164732299</v>
       </c>
       <c r="B323">
-        <v>0.2651488856678822</v>
+        <v>0.1046784168884556</v>
       </c>
     </row>
     <row r="324" spans="1:3">
       <c r="A324">
-        <v>15046.36048854081</v>
+        <v>13761.22494405184</v>
       </c>
       <c r="B324">
-        <v>0.1903702532187453</v>
+        <v>0.02910120499420743</v>
       </c>
     </row>
     <row r="325" spans="1:3">
       <c r="A325">
-        <v>17266.0366188608</v>
+        <v>15547.30484376199</v>
       </c>
       <c r="B325">
-        <v>0.07093168036944786</v>
+        <v>0</v>
+      </c>
+      <c r="C325" s="2">
+        <v>714</v>
       </c>
     </row>
     <row r="326" spans="1:3">
       <c r="A326">
-        <v>17503.9889866208</v>
+        <v>15745.30094133043</v>
       </c>
       <c r="B326">
-        <v>0.05812769927367034</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:3">
       <c r="A327">
-        <v>18508.81984062081</v>
+        <v>16612.01277084961</v>
       </c>
       <c r="B327">
-        <v>0.004058746818250913</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:3">
       <c r="A328">
-        <v>18653.61634614081</v>
+        <v>16740.43210526347</v>
       </c>
       <c r="B328">
         <v>0</v>
-      </c>
-      <c r="C328" s="2">
-        <v>735</v>
       </c>
     </row>
     <row r="329" spans="1:3">
       <c r="A329">
-        <v>18696.4927198208</v>
+        <v>16778.60553209346</v>
       </c>
       <c r="B329">
         <v>0</v>
@@ -3066,7 +3054,7 @@
     </row>
     <row r="330" spans="1:3">
       <c r="A330">
-        <v>19932.71008374081</v>
+        <v>17879.22690086347</v>
       </c>
       <c r="B330">
         <v>0</v>
@@ -3074,7 +3062,7 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331">
-        <v>21801.72729774081</v>
+        <v>19543.23870361347</v>
       </c>
       <c r="B331">
         <v>0</v>
@@ -3082,31 +3070,31 @@
     </row>
     <row r="332" spans="1:3">
       <c r="A332">
-        <v>20619.35388510081</v>
+        <v>18490.55534727346</v>
       </c>
       <c r="B332">
-        <v>0.05423301541628422</v>
+        <v>0.05386432475725567</v>
       </c>
     </row>
     <row r="333" spans="1:3">
       <c r="A333">
-        <v>21411.00244950081</v>
+        <v>19195.37098242347</v>
       </c>
       <c r="B333">
-        <v>0.01792173816798859</v>
+        <v>0.01779990136054987</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334">
-        <v>21064.3878274208</v>
+        <v>18886.77520394347</v>
       </c>
       <c r="B334">
-        <v>0.03382023177569093</v>
+        <v>0.03359031272276392</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335">
-        <v>21870.0347419808</v>
+        <v>19604.05376330347</v>
       </c>
       <c r="B335">
         <v>0</v>
@@ -3117,21 +3105,37 @@
     </row>
     <row r="336" spans="1:3">
       <c r="A336">
-        <v>20794.49238990081</v>
+        <v>18683.7444319692</v>
       </c>
       <c r="B336">
-        <v>0.0491788131463472</v>
+        <v>0.04694484836891144</v>
       </c>
     </row>
     <row r="337" spans="1:3">
       <c r="A337">
-        <v>20794.49238990081</v>
+        <v>18663.82843350585</v>
       </c>
       <c r="B337">
-        <v>0.0491788131463472</v>
-      </c>
-      <c r="C337" s="2">
-        <v>14</v>
+        <v>0.04796076062378563</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338">
+        <v>18721.41054319585</v>
+      </c>
+      <c r="B338">
+        <v>0.04502350538131183</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339">
+        <v>18721.40926566584</v>
+      </c>
+      <c r="B339">
+        <v>0.04502357054793593</v>
+      </c>
+      <c r="C339" s="2">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>